<commit_message>
move file after request created
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.m\Documents\UiPath\HelpDeskTicketGeneration\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5640133-192A-4F29-8E5B-53E57FE0C29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E5FE2F-6422-4149-B9C4-498966FB96A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>RequestFilePath</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>C:\Users\an.m\Documents\UiPath\HelpDeskTicketGeneration\Data\Screenshots\screenshot.png</t>
+  </si>
+  <si>
+    <t>ProcessedFolderPath</t>
+  </si>
+  <si>
+    <t>ProcessedFolderPathEnd</t>
+  </si>
+  <si>
+    <t>UiPath\HelpDeskTicketGeneration\Data\Processed\</t>
   </si>
 </sst>
 </file>
@@ -397,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -445,17 +454,34 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT(B2,B5)</f>
+        <v>C:\Users\an.m\Documents\UiPath\HelpDeskTicketGeneration\Data\Processed\</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>